<commit_message>
Added Data provider support for login
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakes\git\Repo1\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repo1\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9B7972-EFAF-48A9-A7F1-124DB0A8B118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BB2316-FCC4-4266-8BF1-C8143C063611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -138,9 +138,6 @@
     <t>janogsd39</t>
   </si>
   <si>
-    <t>lipmuio29</t>
-  </si>
-  <si>
     <t>xersrtdfokokjuhgyh673</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
   </si>
   <si>
     <t>bhvgfgfyhu123</t>
-  </si>
-  <si>
-    <t>miok98776</t>
   </si>
   <si>
     <t>Feature File
@@ -161,16 +155,48 @@
   </si>
   <si>
     <t>098zwvsa</t>
+  </si>
+  <si>
+    <t>testtttt</t>
+  </si>
+  <si>
+    <t>testttt</t>
+  </si>
+  <si>
+    <t>ytyutu</t>
+  </si>
+  <si>
+    <t>qachamps3</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Ninjatest@123</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -205,6 +231,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3B87CB-D88D-4F0A-BB8F-81BBB5EF62ED}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -693,7 +721,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
@@ -710,7 +738,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
@@ -732,9 +760,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5AF72C-2997-422C-89B0-2C3C703E5609}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -757,7 +785,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,15 +801,45 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new tests for practice page
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -3,37 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DC8B5BB8-5610-40E9-888A-744EF0201E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repo1\src\test\resources\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E202C4E9-F6DD-4F40-97C0-F5D0308370D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
-    <sheet name="Login" sheetId="3" r:id="rId2"/>
+    <sheet name="login" sheetId="3" r:id="rId2"/>
+    <sheet name="pythonCode" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>username</t>
   </si>
@@ -172,13 +166,101 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>pythonCode</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>print("hello");</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>submission success</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,13 +279,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,10 +314,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -229,9 +329,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{DBC3F2C0-FDCB-4F40-91E5-92D8C81EDAEA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3B87CB-D88D-4F0A-BB8F-81BBB5EF62ED}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:B14"/>
     </sheetView>
   </sheetViews>
@@ -759,7 +872,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,4 +954,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C1BB72-E077-4E53-9B8E-2362A02F5343}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added code for practice questions
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repo1\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E202C4E9-F6DD-4F40-97C0-F5D0308370D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C4499E-6B0D-497C-ABB8-143D99B0D42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>username</t>
   </si>
@@ -174,30 +174,27 @@
     <t>Result</t>
   </si>
   <si>
-    <t>print("hello");</t>
-  </si>
-  <si>
-    <t>hello</t>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
   </si>
   <si>
     <t>def search(input_list, num):
 if(num in input_list):
 print("Element Found")
-\b
-\b
+\xc
+\xc
 else:
 print("Not Found")
-\b
-\b
-\b
-\b
+\xc
+\xc
+\xc
+\xc
 search([12, 23, 45, 67, 6, 90] , 12)</t>
-  </si>
-  <si>
-    <t>Element Found</t>
-  </si>
-  <si>
-    <t>submission success</t>
   </si>
   <si>
     <t>def findMaxConsecutiveOnes(nums) :
@@ -206,22 +203,19 @@
 for i in range(0, len(nums)):
 if (nums[i] == 0):
 count = 0
-\b
-\b
+\xc
+\xc
 else:
 count+= 1
-\b
-\b
+\xc
+\xc
 result = max(result, count)
-\b
-\b
+\xc
+\xc
 print(result)
-\b
-\b
+\xc
+\xc
 findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>def findNumbers(nums):
@@ -231,10 +225,10 @@
 x=len(j)
 if x%2==0:
 c=c+1
-\b
-\b
-\b
-\b
+\xc
+\xc
+\xc
+\xc
 print c
 return c
 findNumbers([12,345,2,6,7896])</t>
@@ -245,22 +239,28 @@
 for i in range(0, len(nums)):
 square = nums[i] * nums[i];
 squares_list.append(square)
-\b
-\b
+\xc
+\xc
 sorted_squares_list = sorted(squares_list)
 print sorted_squares_list;
 return sorted_squares_list;
 sortedSquares([-7,-3,2,3,11])</t>
   </si>
   <si>
-    <t>[4, 9, 9, 49, 121]</t>
+    <t xml:space="preserve"> Some Tests failed. Please review code</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No tests were collected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,12 +283,25 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFEBEBEB"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -318,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -329,18 +342,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,7 +695,7 @@
       <selection activeCell="A12" sqref="A12:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
@@ -692,7 +705,7 @@
     <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="48.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -710,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
@@ -718,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -729,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -743,7 +756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -760,7 +773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -777,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -794,7 +807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -811,7 +824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -828,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -845,7 +858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -875,13 +888,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -897,7 +910,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -905,7 +918,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -913,7 +926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -921,7 +934,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -929,13 +942,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="5"/>
       <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -943,7 +956,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
@@ -958,18 +971,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C1BB72-E077-4E53-9B8E-2362A02F5343}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
@@ -977,89 +990,69 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" ht="180">
+      <c r="A2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="180">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="285">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="285">
       <c r="A5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="210">
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="210">
       <c r="A7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="180">
       <c r="A8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="180">
       <c r="A9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>